<commit_message>
Includes front-end JavaScript libraries with known security vulnerabilities-solved
</commit_message>
<xml_diff>
--- a/SEO-audit-Lea Maljkovic.xlsx
+++ b/SEO-audit-Lea Maljkovic.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leazi\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leazi\OneDrive\Desktop\projekt 4\P4-Project-Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24F2F6A9-0C93-4A04-8B68-2D8A08CE868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4537F1A8-1784-46F0-8F3D-913D6DD0F20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Category</t>
   </si>
@@ -193,13 +193,28 @@
   </si>
   <si>
     <t>Put the "&lt;script src="./js/blocs.js"&gt;&lt;/script&gt;&lt;script src="./js/gmaps.js"&gt;&lt;/script&gt;" above the closed tag of &lt;/html&gt;.</t>
+  </si>
+  <si>
+    <t>Hidden Text or Links, keywords stuffing</t>
+  </si>
+  <si>
+    <t>https://www.wordstream.com/black-hat-seo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black hat SEO tecniques are ineffective on modern search engines and the pose a banning risk </t>
+  </si>
+  <si>
+    <t>Always follow search engines guidelines and T&amp;C</t>
+  </si>
+  <si>
+    <t>Black Hat technique present</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,6 +298,13 @@
       <name val="Open Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -318,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -348,6 +370,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -567,13 +591,13 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.23046875" customWidth="1"/>
-    <col min="2" max="2" width="26.921875" customWidth="1"/>
+    <col min="2" max="2" width="28.4609375" customWidth="1"/>
     <col min="3" max="3" width="24.921875" customWidth="1"/>
     <col min="4" max="4" width="25.84375" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
@@ -827,10 +851,28 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="4"/>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="17"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1824,8 +1866,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1" display="https://github.com/terser-js/terser" xr:uid="{C6F5F452-E103-49B4-A4D4-1164DBAC389E}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{D5FB1355-F69D-47AF-BE48-5D59C949557E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>